<commit_message>
Finished experiment 3 and tryid making agent judge more robust
</commit_message>
<xml_diff>
--- a/experiments/experiments_definition.xlsx
+++ b/experiments/experiments_definition.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/i589287/Documents/Repositories/master_thesis/experiments/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ED6400BD-70F0-6947-B173-D7E3F799210C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{037DFD55-4C8F-5347-979F-C5918869A191}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2340" yWindow="7720" windowWidth="28900" windowHeight="18880" xr2:uid="{50CD2D90-D21A-D648-A29F-CF501D2CC0AB}"/>
+    <workbookView xWindow="100" yWindow="760" windowWidth="28900" windowHeight="18880" xr2:uid="{50CD2D90-D21A-D648-A29F-CF501D2CC0AB}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -632,7 +632,7 @@
   <dimension ref="A1:G13"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
-      <selection activeCell="J5" sqref="J5"/>
+      <selection activeCell="H7" sqref="H7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -712,7 +712,7 @@
         <v>1</v>
       </c>
       <c r="G3" s="2" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.2">
@@ -735,7 +735,7 @@
         <v>1</v>
       </c>
       <c r="G4" s="2" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.2">

</xml_diff>